<commit_message>
Added a new template for ExcelImport (Product Prices) -> makes it easier to seperate these from the content Updated the examples
</commit_message>
<xml_diff>
--- a/framework/common/webapp/common/static/product_content_example.xlsx
+++ b/framework/common/webapp/common/static/product_content_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\workspace\jewellerybox\framework\common\webapp\common\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD9DE8-96F2-4FC1-9A26-CB9918E1334F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134C1E64-AB0D-4A3F-8814-FAEFBEBF2A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>altUrl-en</t>
   </si>
@@ -77,12 +77,6 @@
     <t>productName-de</t>
   </si>
   <si>
-    <t>listPrice-EUR</t>
-  </si>
-  <si>
-    <t>defaultPrice-EUR</t>
-  </si>
-  <si>
     <t>PH-1004</t>
   </si>
   <si>
@@ -108,12 +102,6 @@
   </si>
   <si>
     <t>Dies ist mittlerweile das langsamste Telefon, dass man noch finden kann. Aber es ist das mordernste und beste was wir als Demo-Case eingestellt haben</t>
-  </si>
-  <si>
-    <t>219.99</t>
-  </si>
-  <si>
-    <t>175.99</t>
   </si>
 </sst>
 </file>
@@ -955,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -973,7 +961,7 @@
     <col min="12" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1013,52 +1001,40 @@
       <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>